<commit_message>
Add diagrams, Nachdenkzettel & Dokumentation
</commit_message>
<xml_diff>
--- a/Projektnote.xlsx
+++ b/Projektnote.xlsx
@@ -28,7 +28,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,14 +310,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t xml:space="preserve">Vorname</t>
   </si>
   <si>
-    <t xml:space="preserve">Vornamae</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nachname</t>
   </si>
   <si>
@@ -369,7 +366,34 @@
     <t xml:space="preserve">Projekt-Note</t>
   </si>
   <si>
-    <t xml:space="preserve">wip</t>
+    <t xml:space="preserve">Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dh102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PixelJumper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niklas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mäckle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nm067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cazim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cu011</t>
   </si>
   <si>
     <t xml:space="preserve">Aufgabe 1</t>
@@ -571,18 +595,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -648,12 +666,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -720,9 +738,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>746280</xdr:colOff>
+      <xdr:colOff>745920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -731,8 +749,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7296480" y="324360"/>
-          <a:ext cx="4572360" cy="866520"/>
+          <a:off x="7305480" y="324360"/>
+          <a:ext cx="4579560" cy="866160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -817,30 +835,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:R80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,10 +881,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -886,10 +905,10 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -898,63 +917,89 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="3" t="n">
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>40181</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="G2" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="5" t="n">
+      <c r="H2" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M2" s="6" t="n">
-        <v>0</v>
+      <c r="M2" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="7" t="n">
-        <f aca="false">SUM(G2:P2)</f>
+      <c r="P2" s="6" t="n">
+        <f aca="false">SUM(F2:O2)</f>
+        <v>30</v>
+      </c>
+      <c r="R2" s="6" t="n">
+        <f aca="false">VLOOKUP(P2,Notenspiegel!$D$17:$E$47,2,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>40060</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="7" t="n">
-        <f aca="false">VLOOKUP(Q2,Notenspiegel!$D$17:$E$47,2,0)</f>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="G3" s="3" t="n">
         <v>3</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>19</v>
+      <c r="I3" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>3</v>
@@ -966,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N3" s="3" t="n">
         <v>3</v>
@@ -974,33 +1019,42 @@
       <c r="O3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="7" t="n">
-        <f aca="false">SUM(G3:P3)</f>
+      <c r="P3" s="6" t="n">
+        <f aca="false">SUM(F3:O3)</f>
+        <v>30</v>
+      </c>
+      <c r="R3" s="6" t="n">
+        <f aca="false">VLOOKUP(P3,Notenspiegel!$D$17:$E$47,2,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>40064</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="7" t="n">
-        <f aca="false">VLOOKUP(Q3,Notenspiegel!$D$17:$E$47,2,0)</f>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="G4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>19</v>
+      <c r="I4" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="J4" s="3" t="n">
         <v>3</v>
@@ -1012,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N4" s="3" t="n">
         <v>3</v>
@@ -1020,775 +1074,772 @@
       <c r="O4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="7" t="n">
-        <f aca="false">SUM(G4:P4)</f>
-        <v>21</v>
-      </c>
-      <c r="S4" s="7" t="n">
-        <f aca="false">VLOOKUP(Q4,Notenspiegel!$D$17:$E$47,2,0)</f>
-        <v>2.7</v>
+      <c r="P4" s="6" t="n">
+        <f aca="false">SUM(F4:O4)</f>
+        <v>30</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <f aca="false">VLOOKUP(P4,Notenspiegel!$D$17:$E$47,2,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q5" s="7" t="n">
-        <f aca="false">SUM(G5:P5)</f>
-        <v>0</v>
-      </c>
-      <c r="S5" s="7" t="n">
-        <f aca="false">VLOOKUP(Q5,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P5" s="6" t="n">
+        <f aca="false">SUM(F5:O5)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="6" t="n">
+        <f aca="false">VLOOKUP(P5,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q6" s="7" t="n">
-        <f aca="false">SUM(G6:P6)</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="n">
-        <f aca="false">VLOOKUP(Q6,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P6" s="6" t="n">
+        <f aca="false">SUM(F6:O6)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="6" t="n">
+        <f aca="false">VLOOKUP(P6,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q7" s="7" t="n">
-        <f aca="false">SUM(G7:P7)</f>
-        <v>0</v>
-      </c>
-      <c r="S7" s="7" t="n">
-        <f aca="false">VLOOKUP(Q7,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P7" s="6" t="n">
+        <f aca="false">SUM(F7:O7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="6" t="n">
+        <f aca="false">VLOOKUP(P7,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q8" s="7" t="n">
-        <f aca="false">SUM(G8:P8)</f>
-        <v>0</v>
-      </c>
-      <c r="S8" s="7" t="n">
-        <f aca="false">VLOOKUP(Q8,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P8" s="6" t="n">
+        <f aca="false">SUM(F8:O8)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="6" t="n">
+        <f aca="false">VLOOKUP(P8,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q9" s="7" t="n">
-        <f aca="false">SUM(G9:P9)</f>
-        <v>0</v>
-      </c>
-      <c r="S9" s="7" t="n">
-        <f aca="false">VLOOKUP(Q9,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P9" s="6" t="n">
+        <f aca="false">SUM(F9:O9)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="6" t="n">
+        <f aca="false">VLOOKUP(P9,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q10" s="7" t="n">
-        <f aca="false">SUM(G10:P10)</f>
-        <v>0</v>
-      </c>
-      <c r="S10" s="7" t="n">
-        <f aca="false">VLOOKUP(Q10,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P10" s="6" t="n">
+        <f aca="false">SUM(F10:O10)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="6" t="n">
+        <f aca="false">VLOOKUP(P10,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q11" s="7" t="n">
-        <f aca="false">SUM(G11:P11)</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="7" t="n">
-        <f aca="false">VLOOKUP(Q11,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P11" s="6" t="n">
+        <f aca="false">SUM(F11:O11)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="6" t="n">
+        <f aca="false">VLOOKUP(P11,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q12" s="7" t="n">
-        <f aca="false">SUM(G12:P12)</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="7" t="n">
-        <f aca="false">VLOOKUP(Q12,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P12" s="6" t="n">
+        <f aca="false">SUM(F12:O12)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="6" t="n">
+        <f aca="false">VLOOKUP(P12,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q13" s="7" t="n">
-        <f aca="false">SUM(G13:P13)</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="7" t="n">
-        <f aca="false">VLOOKUP(Q13,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P13" s="6" t="n">
+        <f aca="false">SUM(F13:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="6" t="n">
+        <f aca="false">VLOOKUP(P13,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q14" s="7" t="n">
-        <f aca="false">SUM(G14:P14)</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="7" t="n">
-        <f aca="false">VLOOKUP(Q14,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P14" s="6" t="n">
+        <f aca="false">SUM(F14:O14)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="6" t="n">
+        <f aca="false">VLOOKUP(P14,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q15" s="7" t="n">
-        <f aca="false">SUM(G15:P15)</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="7" t="n">
-        <f aca="false">VLOOKUP(Q15,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P15" s="6" t="n">
+        <f aca="false">SUM(F15:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="6" t="n">
+        <f aca="false">VLOOKUP(P15,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q16" s="7" t="n">
-        <f aca="false">SUM(G16:P16)</f>
-        <v>0</v>
-      </c>
-      <c r="S16" s="7" t="n">
-        <f aca="false">VLOOKUP(Q16,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P16" s="6" t="n">
+        <f aca="false">SUM(F16:O16)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="6" t="n">
+        <f aca="false">VLOOKUP(P16,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q17" s="7" t="n">
-        <f aca="false">SUM(G17:P17)</f>
-        <v>0</v>
-      </c>
-      <c r="S17" s="7" t="n">
-        <f aca="false">VLOOKUP(Q17,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P17" s="6" t="n">
+        <f aca="false">SUM(F17:O17)</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="6" t="n">
+        <f aca="false">VLOOKUP(P17,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q18" s="7" t="n">
-        <f aca="false">SUM(G18:P18)</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="7" t="n">
-        <f aca="false">VLOOKUP(Q18,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P18" s="6" t="n">
+        <f aca="false">SUM(F18:O18)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="6" t="n">
+        <f aca="false">VLOOKUP(P18,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q19" s="7" t="n">
-        <f aca="false">SUM(G19:P19)</f>
-        <v>0</v>
-      </c>
-      <c r="S19" s="7" t="n">
-        <f aca="false">VLOOKUP(Q19,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P19" s="6" t="n">
+        <f aca="false">SUM(F19:O19)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="6" t="n">
+        <f aca="false">VLOOKUP(P19,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q20" s="7" t="n">
-        <f aca="false">SUM(G20:P20)</f>
-        <v>0</v>
-      </c>
-      <c r="S20" s="7" t="n">
-        <f aca="false">VLOOKUP(Q20,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P20" s="6" t="n">
+        <f aca="false">SUM(F20:O20)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="6" t="n">
+        <f aca="false">VLOOKUP(P20,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q21" s="7" t="n">
-        <f aca="false">SUM(G21:P21)</f>
-        <v>0</v>
-      </c>
-      <c r="S21" s="7" t="n">
-        <f aca="false">VLOOKUP(Q21,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P21" s="6" t="n">
+        <f aca="false">SUM(F21:O21)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="6" t="n">
+        <f aca="false">VLOOKUP(P21,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q22" s="7" t="n">
-        <f aca="false">SUM(G22:P22)</f>
-        <v>0</v>
-      </c>
-      <c r="S22" s="7" t="n">
-        <f aca="false">VLOOKUP(Q22,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P22" s="6" t="n">
+        <f aca="false">SUM(F22:O22)</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="6" t="n">
+        <f aca="false">VLOOKUP(P22,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q23" s="7" t="n">
-        <f aca="false">SUM(G23:P23)</f>
-        <v>0</v>
-      </c>
-      <c r="S23" s="7" t="n">
-        <f aca="false">VLOOKUP(Q23,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P23" s="6" t="n">
+        <f aca="false">SUM(F23:O23)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="6" t="n">
+        <f aca="false">VLOOKUP(P23,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q24" s="7" t="n">
-        <f aca="false">SUM(G24:P24)</f>
-        <v>0</v>
-      </c>
-      <c r="S24" s="7" t="n">
-        <f aca="false">VLOOKUP(Q24,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P24" s="6" t="n">
+        <f aca="false">SUM(F24:O24)</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="6" t="n">
+        <f aca="false">VLOOKUP(P24,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q25" s="7" t="n">
-        <f aca="false">SUM(G25:P25)</f>
-        <v>0</v>
-      </c>
-      <c r="S25" s="7" t="n">
-        <f aca="false">VLOOKUP(Q25,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P25" s="6" t="n">
+        <f aca="false">SUM(F25:O25)</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="6" t="n">
+        <f aca="false">VLOOKUP(P25,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q26" s="7" t="n">
-        <f aca="false">SUM(G26:P26)</f>
-        <v>0</v>
-      </c>
-      <c r="S26" s="7" t="n">
-        <f aca="false">VLOOKUP(Q26,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P26" s="6" t="n">
+        <f aca="false">SUM(F26:O26)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="6" t="n">
+        <f aca="false">VLOOKUP(P26,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q27" s="7" t="n">
-        <f aca="false">SUM(G27:P27)</f>
-        <v>0</v>
-      </c>
-      <c r="S27" s="7" t="n">
-        <f aca="false">VLOOKUP(Q27,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P27" s="6" t="n">
+        <f aca="false">SUM(F27:O27)</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="6" t="n">
+        <f aca="false">VLOOKUP(P27,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q28" s="7" t="n">
-        <f aca="false">SUM(G28:P28)</f>
-        <v>0</v>
-      </c>
-      <c r="S28" s="7" t="n">
-        <f aca="false">VLOOKUP(Q28,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P28" s="6" t="n">
+        <f aca="false">SUM(F28:O28)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="6" t="n">
+        <f aca="false">VLOOKUP(P28,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q29" s="7" t="n">
-        <f aca="false">SUM(G29:P29)</f>
-        <v>0</v>
-      </c>
-      <c r="S29" s="7" t="n">
-        <f aca="false">VLOOKUP(Q29,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P29" s="6" t="n">
+        <f aca="false">SUM(F29:O29)</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="6" t="n">
+        <f aca="false">VLOOKUP(P29,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q30" s="7" t="n">
-        <f aca="false">SUM(G30:P30)</f>
-        <v>0</v>
-      </c>
-      <c r="S30" s="7" t="n">
-        <f aca="false">VLOOKUP(Q30,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P30" s="6" t="n">
+        <f aca="false">SUM(F30:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="6" t="n">
+        <f aca="false">VLOOKUP(P30,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q31" s="7" t="n">
-        <f aca="false">SUM(G31:P31)</f>
-        <v>0</v>
-      </c>
-      <c r="S31" s="7" t="n">
-        <f aca="false">VLOOKUP(Q31,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P31" s="6" t="n">
+        <f aca="false">SUM(F31:O31)</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="6" t="n">
+        <f aca="false">VLOOKUP(P31,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q32" s="7" t="n">
-        <f aca="false">SUM(G32:P32)</f>
-        <v>0</v>
-      </c>
-      <c r="S32" s="7" t="n">
-        <f aca="false">VLOOKUP(Q32,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P32" s="6" t="n">
+        <f aca="false">SUM(F32:O32)</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="6" t="n">
+        <f aca="false">VLOOKUP(P32,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q33" s="7" t="n">
-        <f aca="false">SUM(G33:P33)</f>
-        <v>0</v>
-      </c>
-      <c r="S33" s="7" t="n">
-        <f aca="false">VLOOKUP(Q33,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P33" s="6" t="n">
+        <f aca="false">SUM(F33:O33)</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="6" t="n">
+        <f aca="false">VLOOKUP(P33,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q34" s="7" t="n">
-        <f aca="false">SUM(G34:P34)</f>
-        <v>0</v>
-      </c>
-      <c r="S34" s="7" t="n">
-        <f aca="false">VLOOKUP(Q34,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P34" s="6" t="n">
+        <f aca="false">SUM(F34:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="6" t="n">
+        <f aca="false">VLOOKUP(P34,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q35" s="7" t="n">
-        <f aca="false">SUM(G35:P35)</f>
-        <v>0</v>
-      </c>
-      <c r="S35" s="7" t="n">
-        <f aca="false">VLOOKUP(Q35,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P35" s="6" t="n">
+        <f aca="false">SUM(F35:O35)</f>
+        <v>0</v>
+      </c>
+      <c r="R35" s="6" t="n">
+        <f aca="false">VLOOKUP(P35,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q36" s="7" t="n">
-        <f aca="false">SUM(G36:P36)</f>
-        <v>0</v>
-      </c>
-      <c r="S36" s="7" t="n">
-        <f aca="false">VLOOKUP(Q36,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P36" s="6" t="n">
+        <f aca="false">SUM(F36:O36)</f>
+        <v>0</v>
+      </c>
+      <c r="R36" s="6" t="n">
+        <f aca="false">VLOOKUP(P36,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q37" s="7" t="n">
-        <f aca="false">SUM(G37:P37)</f>
-        <v>0</v>
-      </c>
-      <c r="S37" s="7" t="n">
-        <f aca="false">VLOOKUP(Q37,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P37" s="6" t="n">
+        <f aca="false">SUM(F37:O37)</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="6" t="n">
+        <f aca="false">VLOOKUP(P37,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q38" s="7" t="n">
-        <f aca="false">SUM(G38:P38)</f>
-        <v>0</v>
-      </c>
-      <c r="S38" s="7" t="n">
-        <f aca="false">VLOOKUP(Q38,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P38" s="6" t="n">
+        <f aca="false">SUM(F38:O38)</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="6" t="n">
+        <f aca="false">VLOOKUP(P38,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q39" s="7" t="n">
-        <f aca="false">SUM(G39:P39)</f>
-        <v>0</v>
-      </c>
-      <c r="S39" s="7" t="n">
-        <f aca="false">VLOOKUP(Q39,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P39" s="6" t="n">
+        <f aca="false">SUM(F39:O39)</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="6" t="n">
+        <f aca="false">VLOOKUP(P39,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q40" s="7" t="n">
-        <f aca="false">SUM(G40:P40)</f>
-        <v>0</v>
-      </c>
-      <c r="S40" s="7" t="n">
-        <f aca="false">VLOOKUP(Q40,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P40" s="6" t="n">
+        <f aca="false">SUM(F40:O40)</f>
+        <v>0</v>
+      </c>
+      <c r="R40" s="6" t="n">
+        <f aca="false">VLOOKUP(P40,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q41" s="7" t="n">
-        <f aca="false">SUM(G41:P41)</f>
-        <v>0</v>
-      </c>
-      <c r="S41" s="7" t="n">
-        <f aca="false">VLOOKUP(Q41,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P41" s="6" t="n">
+        <f aca="false">SUM(F41:O41)</f>
+        <v>0</v>
+      </c>
+      <c r="R41" s="6" t="n">
+        <f aca="false">VLOOKUP(P41,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q42" s="7" t="n">
-        <f aca="false">SUM(G42:P42)</f>
-        <v>0</v>
-      </c>
-      <c r="S42" s="7" t="n">
-        <f aca="false">VLOOKUP(Q42,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P42" s="6" t="n">
+        <f aca="false">SUM(F42:O42)</f>
+        <v>0</v>
+      </c>
+      <c r="R42" s="6" t="n">
+        <f aca="false">VLOOKUP(P42,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q43" s="7" t="n">
-        <f aca="false">SUM(G43:P43)</f>
-        <v>0</v>
-      </c>
-      <c r="S43" s="7" t="n">
-        <f aca="false">VLOOKUP(Q43,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P43" s="6" t="n">
+        <f aca="false">SUM(F43:O43)</f>
+        <v>0</v>
+      </c>
+      <c r="R43" s="6" t="n">
+        <f aca="false">VLOOKUP(P43,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q44" s="7" t="n">
-        <f aca="false">SUM(G44:P44)</f>
-        <v>0</v>
-      </c>
-      <c r="S44" s="7" t="n">
-        <f aca="false">VLOOKUP(Q44,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P44" s="6" t="n">
+        <f aca="false">SUM(F44:O44)</f>
+        <v>0</v>
+      </c>
+      <c r="R44" s="6" t="n">
+        <f aca="false">VLOOKUP(P44,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q45" s="7" t="n">
-        <f aca="false">SUM(G45:P45)</f>
-        <v>0</v>
-      </c>
-      <c r="S45" s="7" t="n">
-        <f aca="false">VLOOKUP(Q45,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P45" s="6" t="n">
+        <f aca="false">SUM(F45:O45)</f>
+        <v>0</v>
+      </c>
+      <c r="R45" s="6" t="n">
+        <f aca="false">VLOOKUP(P45,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q46" s="7" t="n">
-        <f aca="false">SUM(G46:P46)</f>
-        <v>0</v>
-      </c>
-      <c r="S46" s="7" t="n">
-        <f aca="false">VLOOKUP(Q46,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P46" s="6" t="n">
+        <f aca="false">SUM(F46:O46)</f>
+        <v>0</v>
+      </c>
+      <c r="R46" s="6" t="n">
+        <f aca="false">VLOOKUP(P46,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q47" s="7" t="n">
-        <f aca="false">SUM(G47:P47)</f>
-        <v>0</v>
-      </c>
-      <c r="S47" s="7" t="n">
-        <f aca="false">VLOOKUP(Q47,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P47" s="6" t="n">
+        <f aca="false">SUM(F47:O47)</f>
+        <v>0</v>
+      </c>
+      <c r="R47" s="6" t="n">
+        <f aca="false">VLOOKUP(P47,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q48" s="7" t="n">
-        <f aca="false">SUM(G48:P48)</f>
-        <v>0</v>
-      </c>
-      <c r="S48" s="7" t="n">
-        <f aca="false">VLOOKUP(Q48,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P48" s="6" t="n">
+        <f aca="false">SUM(F48:O48)</f>
+        <v>0</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <f aca="false">VLOOKUP(P48,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q49" s="7" t="n">
-        <f aca="false">SUM(G49:P49)</f>
-        <v>0</v>
-      </c>
-      <c r="S49" s="7" t="n">
-        <f aca="false">VLOOKUP(Q49,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P49" s="6" t="n">
+        <f aca="false">SUM(F49:O49)</f>
+        <v>0</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <f aca="false">VLOOKUP(P49,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q50" s="7" t="n">
-        <f aca="false">SUM(G50:P50)</f>
-        <v>0</v>
-      </c>
-      <c r="S50" s="7" t="n">
-        <f aca="false">VLOOKUP(Q50,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P50" s="6" t="n">
+        <f aca="false">SUM(F50:O50)</f>
+        <v>0</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <f aca="false">VLOOKUP(P50,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q51" s="7" t="n">
-        <f aca="false">SUM(G51:P51)</f>
-        <v>0</v>
-      </c>
-      <c r="S51" s="7" t="n">
-        <f aca="false">VLOOKUP(Q51,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P51" s="6" t="n">
+        <f aca="false">SUM(F51:O51)</f>
+        <v>0</v>
+      </c>
+      <c r="R51" s="6" t="n">
+        <f aca="false">VLOOKUP(P51,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q52" s="7" t="n">
-        <f aca="false">SUM(G52:P52)</f>
-        <v>0</v>
-      </c>
-      <c r="S52" s="7" t="n">
-        <f aca="false">VLOOKUP(Q52,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P52" s="6" t="n">
+        <f aca="false">SUM(F52:O52)</f>
+        <v>0</v>
+      </c>
+      <c r="R52" s="6" t="n">
+        <f aca="false">VLOOKUP(P52,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q53" s="7" t="n">
-        <f aca="false">SUM(G53:P53)</f>
-        <v>0</v>
-      </c>
-      <c r="S53" s="7" t="n">
-        <f aca="false">VLOOKUP(Q53,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P53" s="6" t="n">
+        <f aca="false">SUM(F53:O53)</f>
+        <v>0</v>
+      </c>
+      <c r="R53" s="6" t="n">
+        <f aca="false">VLOOKUP(P53,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q54" s="7" t="n">
-        <f aca="false">SUM(G54:P54)</f>
-        <v>0</v>
-      </c>
-      <c r="S54" s="7" t="n">
-        <f aca="false">VLOOKUP(Q54,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P54" s="6" t="n">
+        <f aca="false">SUM(F54:O54)</f>
+        <v>0</v>
+      </c>
+      <c r="R54" s="6" t="n">
+        <f aca="false">VLOOKUP(P54,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q55" s="7" t="n">
-        <f aca="false">SUM(G55:P55)</f>
-        <v>0</v>
-      </c>
-      <c r="S55" s="7" t="n">
-        <f aca="false">VLOOKUP(Q55,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P55" s="6" t="n">
+        <f aca="false">SUM(F55:O55)</f>
+        <v>0</v>
+      </c>
+      <c r="R55" s="6" t="n">
+        <f aca="false">VLOOKUP(P55,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q56" s="7" t="n">
-        <f aca="false">SUM(G56:P56)</f>
-        <v>0</v>
-      </c>
-      <c r="S56" s="7" t="n">
-        <f aca="false">VLOOKUP(Q56,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P56" s="6" t="n">
+        <f aca="false">SUM(F56:O56)</f>
+        <v>0</v>
+      </c>
+      <c r="R56" s="6" t="n">
+        <f aca="false">VLOOKUP(P56,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q57" s="7" t="n">
-        <f aca="false">SUM(G57:P57)</f>
-        <v>0</v>
-      </c>
-      <c r="S57" s="7" t="n">
-        <f aca="false">VLOOKUP(Q57,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P57" s="6" t="n">
+        <f aca="false">SUM(F57:O57)</f>
+        <v>0</v>
+      </c>
+      <c r="R57" s="6" t="n">
+        <f aca="false">VLOOKUP(P57,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q58" s="7" t="n">
-        <f aca="false">SUM(G58:P58)</f>
-        <v>0</v>
-      </c>
-      <c r="S58" s="7" t="n">
-        <f aca="false">VLOOKUP(Q58,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P58" s="6" t="n">
+        <f aca="false">SUM(F58:O58)</f>
+        <v>0</v>
+      </c>
+      <c r="R58" s="6" t="n">
+        <f aca="false">VLOOKUP(P58,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q59" s="7" t="n">
-        <f aca="false">SUM(G59:P59)</f>
-        <v>0</v>
-      </c>
-      <c r="S59" s="7" t="n">
-        <f aca="false">VLOOKUP(Q59,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P59" s="6" t="n">
+        <f aca="false">SUM(F59:O59)</f>
+        <v>0</v>
+      </c>
+      <c r="R59" s="6" t="n">
+        <f aca="false">VLOOKUP(P59,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q60" s="7" t="n">
-        <f aca="false">SUM(G60:P60)</f>
-        <v>0</v>
-      </c>
-      <c r="S60" s="7" t="n">
-        <f aca="false">VLOOKUP(Q60,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P60" s="6" t="n">
+        <f aca="false">SUM(F60:O60)</f>
+        <v>0</v>
+      </c>
+      <c r="R60" s="6" t="n">
+        <f aca="false">VLOOKUP(P60,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q61" s="7" t="n">
-        <f aca="false">SUM(G61:P61)</f>
-        <v>0</v>
-      </c>
-      <c r="S61" s="7" t="n">
-        <f aca="false">VLOOKUP(Q61,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P61" s="6" t="n">
+        <f aca="false">SUM(F61:O61)</f>
+        <v>0</v>
+      </c>
+      <c r="R61" s="6" t="n">
+        <f aca="false">VLOOKUP(P61,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q62" s="7" t="n">
-        <f aca="false">SUM(G62:P62)</f>
-        <v>0</v>
-      </c>
-      <c r="S62" s="7" t="n">
-        <f aca="false">VLOOKUP(Q62,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P62" s="6" t="n">
+        <f aca="false">SUM(F62:O62)</f>
+        <v>0</v>
+      </c>
+      <c r="R62" s="6" t="n">
+        <f aca="false">VLOOKUP(P62,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q63" s="7" t="n">
-        <f aca="false">SUM(G63:P63)</f>
-        <v>0</v>
-      </c>
-      <c r="S63" s="7" t="n">
-        <f aca="false">VLOOKUP(Q63,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P63" s="6" t="n">
+        <f aca="false">SUM(F63:O63)</f>
+        <v>0</v>
+      </c>
+      <c r="R63" s="6" t="n">
+        <f aca="false">VLOOKUP(P63,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q64" s="7" t="n">
-        <f aca="false">SUM(G64:P64)</f>
-        <v>0</v>
-      </c>
-      <c r="S64" s="7" t="n">
-        <f aca="false">VLOOKUP(Q64,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P64" s="6" t="n">
+        <f aca="false">SUM(F64:O64)</f>
+        <v>0</v>
+      </c>
+      <c r="R64" s="6" t="n">
+        <f aca="false">VLOOKUP(P64,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q65" s="7" t="n">
-        <f aca="false">SUM(G65:P65)</f>
-        <v>0</v>
-      </c>
-      <c r="S65" s="7" t="n">
-        <f aca="false">VLOOKUP(Q65,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P65" s="6" t="n">
+        <f aca="false">SUM(F65:O65)</f>
+        <v>0</v>
+      </c>
+      <c r="R65" s="6" t="n">
+        <f aca="false">VLOOKUP(P65,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q66" s="7" t="n">
-        <f aca="false">SUM(G66:P66)</f>
-        <v>0</v>
-      </c>
-      <c r="S66" s="7" t="n">
-        <f aca="false">VLOOKUP(Q66,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P66" s="6" t="n">
+        <f aca="false">SUM(F66:O66)</f>
+        <v>0</v>
+      </c>
+      <c r="R66" s="6" t="n">
+        <f aca="false">VLOOKUP(P66,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q67" s="7" t="n">
-        <f aca="false">SUM(G67:P67)</f>
-        <v>0</v>
-      </c>
-      <c r="S67" s="7" t="n">
-        <f aca="false">VLOOKUP(Q67,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P67" s="6" t="n">
+        <f aca="false">SUM(F67:O67)</f>
+        <v>0</v>
+      </c>
+      <c r="R67" s="6" t="n">
+        <f aca="false">VLOOKUP(P67,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q68" s="7" t="n">
-        <f aca="false">SUM(G68:P68)</f>
-        <v>0</v>
-      </c>
-      <c r="S68" s="7" t="n">
-        <f aca="false">VLOOKUP(Q68,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P68" s="6" t="n">
+        <f aca="false">SUM(F68:O68)</f>
+        <v>0</v>
+      </c>
+      <c r="R68" s="6" t="n">
+        <f aca="false">VLOOKUP(P68,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q69" s="7" t="n">
-        <f aca="false">SUM(G69:P69)</f>
-        <v>0</v>
-      </c>
-      <c r="S69" s="7" t="n">
-        <f aca="false">VLOOKUP(Q69,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P69" s="6" t="n">
+        <f aca="false">SUM(F69:O69)</f>
+        <v>0</v>
+      </c>
+      <c r="R69" s="6" t="n">
+        <f aca="false">VLOOKUP(P69,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q70" s="7" t="n">
-        <f aca="false">SUM(G70:P70)</f>
-        <v>0</v>
-      </c>
-      <c r="S70" s="7" t="n">
-        <f aca="false">VLOOKUP(Q70,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P70" s="6" t="n">
+        <f aca="false">SUM(F70:O70)</f>
+        <v>0</v>
+      </c>
+      <c r="R70" s="6" t="n">
+        <f aca="false">VLOOKUP(P70,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q71" s="7" t="n">
-        <f aca="false">SUM(G71:P71)</f>
-        <v>0</v>
-      </c>
-      <c r="S71" s="7" t="n">
-        <f aca="false">VLOOKUP(Q71,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P71" s="6" t="n">
+        <f aca="false">SUM(F71:O71)</f>
+        <v>0</v>
+      </c>
+      <c r="R71" s="6" t="n">
+        <f aca="false">VLOOKUP(P71,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q72" s="7" t="n">
-        <f aca="false">SUM(G72:P72)</f>
-        <v>0</v>
-      </c>
-      <c r="S72" s="7" t="n">
-        <f aca="false">VLOOKUP(Q72,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P72" s="6" t="n">
+        <f aca="false">SUM(F72:O72)</f>
+        <v>0</v>
+      </c>
+      <c r="R72" s="6" t="n">
+        <f aca="false">VLOOKUP(P72,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q73" s="7" t="n">
-        <f aca="false">SUM(G73:P73)</f>
-        <v>0</v>
-      </c>
-      <c r="S73" s="7" t="n">
-        <f aca="false">VLOOKUP(Q73,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P73" s="6" t="n">
+        <f aca="false">SUM(F73:O73)</f>
+        <v>0</v>
+      </c>
+      <c r="R73" s="6" t="n">
+        <f aca="false">VLOOKUP(P73,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q74" s="7" t="n">
-        <f aca="false">SUM(G74:P74)</f>
-        <v>0</v>
-      </c>
-      <c r="S74" s="7" t="n">
-        <f aca="false">VLOOKUP(Q74,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P74" s="6" t="n">
+        <f aca="false">SUM(F74:O74)</f>
+        <v>0</v>
+      </c>
+      <c r="R74" s="6" t="n">
+        <f aca="false">VLOOKUP(P74,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q75" s="7" t="n">
-        <f aca="false">SUM(G75:P75)</f>
-        <v>0</v>
-      </c>
-      <c r="S75" s="7" t="n">
-        <f aca="false">VLOOKUP(Q75,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P75" s="6" t="n">
+        <f aca="false">SUM(F75:O75)</f>
+        <v>0</v>
+      </c>
+      <c r="R75" s="6" t="n">
+        <f aca="false">VLOOKUP(P75,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q76" s="7" t="n">
-        <f aca="false">SUM(G76:P76)</f>
-        <v>0</v>
-      </c>
-      <c r="S76" s="7" t="n">
-        <f aca="false">VLOOKUP(Q76,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P76" s="6" t="n">
+        <f aca="false">SUM(F76:O76)</f>
+        <v>0</v>
+      </c>
+      <c r="R76" s="6" t="n">
+        <f aca="false">VLOOKUP(P76,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q77" s="7" t="n">
-        <f aca="false">SUM(G77:P77)</f>
-        <v>0</v>
-      </c>
-      <c r="S77" s="7" t="n">
-        <f aca="false">VLOOKUP(Q77,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P77" s="6" t="n">
+        <f aca="false">SUM(F77:O77)</f>
+        <v>0</v>
+      </c>
+      <c r="R77" s="6" t="n">
+        <f aca="false">VLOOKUP(P77,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q78" s="7" t="n">
-        <f aca="false">SUM(G78:P78)</f>
-        <v>0</v>
-      </c>
-      <c r="S78" s="7" t="n">
-        <f aca="false">VLOOKUP(Q78,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P78" s="6" t="n">
+        <f aca="false">SUM(F78:O78)</f>
+        <v>0</v>
+      </c>
+      <c r="R78" s="6" t="n">
+        <f aca="false">VLOOKUP(P78,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q79" s="7" t="n">
-        <f aca="false">SUM(G79:P79)</f>
-        <v>0</v>
-      </c>
-      <c r="S79" s="7" t="n">
-        <f aca="false">VLOOKUP(Q79,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P79" s="6" t="n">
+        <f aca="false">SUM(F79:O79)</f>
+        <v>0</v>
+      </c>
+      <c r="R79" s="6" t="n">
+        <f aca="false">VLOOKUP(P79,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q80" s="7" t="n">
-        <f aca="false">SUM(G80:P80)</f>
-        <v>0</v>
-      </c>
-      <c r="S80" s="7" t="n">
-        <f aca="false">VLOOKUP(Q80,Notenspiegel!$D$17:$E$47,2,0)</f>
+      <c r="P80" s="6" t="n">
+        <f aca="false">SUM(F80:O80)</f>
+        <v>0</v>
+      </c>
+      <c r="R80" s="6" t="n">
+        <f aca="false">VLOOKUP(P80,Notenspiegel!$D$17:$E$47,2,0)</f>
         <v>5</v>
       </c>
     </row>
@@ -1815,7 +1866,7 @@
       <selection pane="topLeft" activeCell="R29" activeCellId="0" sqref="R29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.19"/>
   </cols>
@@ -1825,49 +1876,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,7 +2723,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.13"/>
   </cols>
@@ -2682,22 +2733,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,22 +3248,22 @@
       <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
@@ -3231,40 +3282,40 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B4" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E4" s="13" t="n">
         <v>1</v>
@@ -3283,14 +3334,14 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>1.3</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="14" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E5" s="13" t="n">
         <v>1.3</v>
@@ -3309,14 +3360,14 @@
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B6" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="14" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E6" s="13" t="n">
         <v>1.7</v>
@@ -3335,7 +3386,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7" s="13" t="n">
         <v>2</v>
@@ -3361,7 +3412,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8" s="13" t="n">
         <v>2.3</v>
@@ -3387,14 +3438,14 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B9" s="13" t="n">
         <v>2.7</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E9" s="13" t="n">
         <v>2.7</v>
@@ -3413,7 +3464,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B10" s="13" t="n">
         <v>3</v>
@@ -3439,14 +3490,14 @@
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B11" s="13" t="n">
         <v>3.3</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="14" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E11" s="13" t="n">
         <v>3.3</v>
@@ -3465,7 +3516,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B12" s="13" t="n">
         <v>3.7</v>
@@ -3491,14 +3542,14 @@
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B13" s="13" t="n">
         <v>4</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="14" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E13" s="13" t="n">
         <v>4</v>
@@ -3517,14 +3568,14 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B14" s="13" t="n">
         <v>4.7</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="17" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E14" s="13" t="n">
         <v>4.7</v>
@@ -3543,14 +3594,14 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B15" s="13" t="n">
         <v>5</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="17" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E15" s="13" t="n">
         <v>5</v>

</xml_diff>